<commit_message>
update chromedriver-136, add cofig properties file
</commit_message>
<xml_diff>
--- a/src/test/resources/report_demo.xlsx
+++ b/src/test/resources/report_demo.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="137">
   <si>
     <t>ID Test Case</t>
   </si>
@@ -492,6 +492,9 @@
   </si>
   <si>
     <t>Holding</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -1142,7 +1145,7 @@
         <v>95</v>
       </c>
       <c r="L4" t="s" s="0">
-        <v>99</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="51" x14ac:dyDescent="0.35">
@@ -1178,7 +1181,7 @@
         <v>95</v>
       </c>
       <c r="L5" t="s" s="0">
-        <v>99</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
@@ -1214,7 +1217,7 @@
         <v>95</v>
       </c>
       <c r="L6" t="s" s="0">
-        <v>99</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
add config screenCapture after check TCs
</commit_message>
<xml_diff>
--- a/src/test/resources/report_demo.xlsx
+++ b/src/test/resources/report_demo.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="137">
   <si>
     <t>ID Test Case</t>
   </si>
@@ -1145,7 +1145,7 @@
         <v>95</v>
       </c>
       <c r="L4" t="s" s="0">
-        <v>136</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="51" x14ac:dyDescent="0.35">
@@ -1181,7 +1181,7 @@
         <v>95</v>
       </c>
       <c r="L5" t="s" s="0">
-        <v>136</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
@@ -1217,7 +1217,7 @@
         <v>95</v>
       </c>
       <c r="L6" t="s" s="0">
-        <v>136</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
add page TimeSheet and TC check table of TimeSheetPage
</commit_message>
<xml_diff>
--- a/src/test/resources/report_demo.xlsx
+++ b/src/test/resources/report_demo.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tester\ProjectHRM\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\test\Selenium\Selenium-Java\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB005C19-4928-4BEF-AC96-6DD50938C695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C26A9030-10AB-4EBC-82F1-A1AEA08DFDA7}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Change_Language" sheetId="2" r:id="rId2"/>
+    <sheet name="Table" sheetId="3" r:id="rId2"/>
+    <sheet name="Change_Language" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Login!$A$1:$M$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="224">
   <si>
     <t>ID Test Case</t>
   </si>
@@ -494,14 +494,274 @@
     <t>Holding</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <t>Data Table / Search &amp; Filter</t>
+  </si>
+  <si>
+    <t>Verify Search Button without Filters</t>
+  </si>
+  <si>
+    <t>Check if clicking Search with no filters applied shows default data</t>
+  </si>
+  <si>
+    <t>User is on the page with the data table.</t>
+  </si>
+  <si>
+    <t>No filter applied.</t>
+  </si>
+  <si>
+    <t>1. Ensure all filter fields (Start Date, End Date, Employee) are empty or default ("All"). &gt; 2. Click the Search button (magnifying glass icon). &gt; 3. Wait for the table to update.</t>
+  </si>
+  <si>
+    <t>Need locators for Search button. Verify initial state of filters. Need a way to check if the table is loaded with data (e.g., check number of rows &gt; 0).</t>
+  </si>
+  <si>
+    <t>The table displays the default set of data (likely all available entries or the initial loaded page).</t>
+  </si>
+  <si>
+    <t>Verify Reset Button</t>
+  </si>
+  <si>
+    <t>Check if clicking Reset clears all filters and shows default data</t>
+  </si>
+  <si>
+    <t>User is on the page with the data table, with some filters applied.</t>
+  </si>
+  <si>
+    <t>Any filters applied (e.g., Start Date, End Date, Employee selected).</t>
+  </si>
+  <si>
+    <t>1. Apply some filters (e.g., select an Employee). &gt; 2. Click the Reset button (circular arrow icon). &gt; 3. Wait for the filters to clear and the table to update.</t>
+  </si>
+  <si>
+    <t>Need locators for Reset button and filter fields to verify they are cleared. Need to verify the table state returns to default.</t>
+  </si>
+  <si>
+    <t>All filter fields (Start Date, End Date, Employee dropdown) are cleared/reset to default, and the table displays the default set of data.</t>
+  </si>
+  <si>
+    <t>Filter by Employee (Specific)</t>
+  </si>
+  <si>
+    <t>Verify filtering by a specific employee shows only their data</t>
+  </si>
+  <si>
+    <t>Specific Employee Name (e.g., "Julie workdo")</t>
+  </si>
+  <si>
+    <t>1. Click the Employee dropdown. &gt; 2. Select a specific employee name from the list (e.g., "Julie workdo"). &gt; 3. Click the Search button. &gt; 4. Wait for the table to update. &gt; 5. Verify results in the table.</t>
+  </si>
+  <si>
+    <t>Need locators for Employee dropdown, dropdown options (can be dynamic), and Search button. Need to iterate through table rows/cells to verify only the selected employee name appears in the "Employee" column.</t>
+  </si>
+  <si>
+    <t>The table is updated to display only entries where the "Employee" column matches the selected employee name.</t>
+  </si>
+  <si>
+    <t>Filter by Employee (All)</t>
+  </si>
+  <si>
+    <t>Verify selecting "All" in Employee dropdown shows all data</t>
+  </si>
+  <si>
+    <t>Employee: "All"</t>
+  </si>
+  <si>
+    <t>1. Click the Employee dropdown. &gt; 2. Select "All" from the list. &gt; 3. Click the Search button. &gt; 4. Wait for the table to update.</t>
+  </si>
+  <si>
+    <t>Need locators for Employee dropdown, "All" option, and Search button. Verify table displays all default data (similar to TC 21).</t>
+  </si>
+  <si>
+    <t>The table is updated to display entries for all employees (default view).</t>
+  </si>
+  <si>
+    <t>Filter by Date Range (Start &amp; End)</t>
+  </si>
+  <si>
+    <t>Verify filtering by a valid date range shows data within that range</t>
+  </si>
+  <si>
+    <t>Start Date: [Date A], End Date: [Date B] (where A &lt;= B and data exists in range)</t>
+  </si>
+  <si>
+    <t>1. Enter [Date A] into the Start Date field. &gt; 2. Enter [Date B] into the End Date field. &gt; 3. Click the Search button. &gt; 4. Wait for the table to update. &gt; 5. Verify results in the table.</t>
+  </si>
+  <si>
+    <t>Need locators for Start Date, End Date fields, and Search button. Need to verify the "Date" column of all displayed rows falls within the [Date A] to [Date B] range. Handling calendar picker automation might be complex.</t>
+  </si>
+  <si>
+    <t>The table is updated to display only entries where the "Date" column is between or equal to the Start Date and End Date.</t>
+  </si>
+  <si>
+    <t>Filter by Start Date Only</t>
+  </si>
+  <si>
+    <t>Verify filtering by only a Start Date shows data from that date onwards</t>
+  </si>
+  <si>
+    <t>Start Date: [Date A], End Date: Empty</t>
+  </si>
+  <si>
+    <t>1. Enter [Date A] into the Start Date field. &gt; 2. Ensure End Date field is empty. &gt; 3. Click the Search button. &gt; 4. Wait for the table to update. &gt; 5. Verify results in the table.</t>
+  </si>
+  <si>
+    <t>Need locators for Start Date, End Date fields, and Search button. Verify the "Date" column of all displayed rows is on or after [Date A].</t>
+  </si>
+  <si>
+    <t>The table is updated to display only entries where the "Date" column is on or after the Start Date.</t>
+  </si>
+  <si>
+    <t>Filter by End Date Only</t>
+  </si>
+  <si>
+    <t>Verify filtering by only an End Date shows data up to that date</t>
+  </si>
+  <si>
+    <t>Start Date: Empty, End Date: [Date B]</t>
+  </si>
+  <si>
+    <t>1. Ensure Start Date field is empty. &gt; 2. Enter [Date B] into the End Date field. &gt; 3. Click the Search button. &gt; 4. Wait for the table to update. &gt; 5. Verify results in the table.</t>
+  </si>
+  <si>
+    <t>Need locators for Start Date, End Date fields, and Search button. Verify the "Date" column of all displayed rows is on or before [Date B].</t>
+  </si>
+  <si>
+    <t>The table is updated to display only entries where the "Date" column is on or before the End Date.</t>
+  </si>
+  <si>
+    <t>Filter by Invalid Date Range (Start &gt; End)</t>
+  </si>
+  <si>
+    <t>Verify appropriate handling when Start Date is after End Date</t>
+  </si>
+  <si>
+    <t>Start Date: [Date A], End Date: [Date B] (where A &gt; B)</t>
+  </si>
+  <si>
+    <t>1. Enter [Date A] into the Start Date field (A &gt; B). &gt; 2. Enter [Date B] into the End Date field (A &gt; B). &gt; 3. Click the Search button. &gt; 4. Wait for the table to update.</t>
+  </si>
+  <si>
+    <t>Need locators for date fields and Search button. Observe UI behavior.</t>
+  </si>
+  <si>
+    <t>The system handles the invalid range (e.g., displays an error message, shows no results, or defaults to no filter). The table should not show data from the invalid range.</t>
+  </si>
+  <si>
+    <t>Filter by Employee and Date Range (Combined)</t>
+  </si>
+  <si>
+    <t>Verify filtering by both employee and date range works correctly</t>
+  </si>
+  <si>
+    <t>Specific Employee Name, Start Date: [Date A], End Date: [Date B]</t>
+  </si>
+  <si>
+    <t>1. Select a specific employee. &gt; 2. Enter [Date A] into Start Date. &gt; 3. Enter [Date B] into End Date. &gt; 4. Click Search. &gt; 5. Wait for table. &gt; 6. Verify results.</t>
+  </si>
+  <si>
+    <t>Need locators for all filter elements. Verify table rows match both the selected employee and the date range.</t>
+  </si>
+  <si>
+    <t>The table is updated to display only entries matching both the selected Employee AND falling within the specified Date Range.</t>
+  </si>
+  <si>
+    <t>General Table Search (by Keyword)</t>
+  </si>
+  <si>
+    <t>Verify the "Search..." box filters table rows based on keyword across columns</t>
+  </si>
+  <si>
+    <t>Keyword string (e.g., part of Employee name or Remark)</t>
+  </si>
+  <si>
+    <t>1. Enter a keyword into the "Search..." input box. &gt; 2. Wait for the table to filter (often happens automatically or requires Enter). &gt; 3. Verify results in the table.</t>
+  </si>
+  <si>
+    <t>Need locator for the "Search..." input box. Verify table rows contain the keyword in any searchable column. Be aware if filtering is instant or requires 'Enter'.</t>
+  </si>
+  <si>
+    <t>The table is filtered to show only rows where at least one searchable column (Employee, Remark, etc.) contains the entered keyword.</t>
+  </si>
+  <si>
+    <t>Clear General Table Search</t>
+  </si>
+  <si>
+    <t>Verify clearing the "Search..." box removes the filter</t>
+  </si>
+  <si>
+    <t>User is on the page with the data table, currently filtered by the "Search..." box.</t>
+  </si>
+  <si>
+    <t>Empty String ("")</t>
+  </si>
+  <si>
+    <t>1. Enter a keyword into the "Search..." input box to apply a filter. &gt; 2. Clear the text in the "Search..." input box. &gt; 3. Wait for the table to update. &gt; 4. Verify results.</t>
+  </si>
+  <si>
+    <t>Need locator for the "Search..." box. Verify table reverts to its state before the general search was applied (either showing all data if no other filters, or showing data based on Start/End/Employee filters).</t>
+  </si>
+  <si>
+    <t>The table filter applied by the "Search..." box is removed, and the table displays data based on the Start Date, End Date, and Employee filters (or all data if those filters are clear).</t>
+  </si>
+  <si>
+    <t>Filter by Non-existent Employee</t>
+  </si>
+  <si>
+    <t>Verify filtering by an employee not in the list or with no data shows no results</t>
+  </si>
+  <si>
+    <t>Non-existent Employee Name</t>
+  </si>
+  <si>
+    <t>1. Select a non-existent employee (if dropdown allows manual entry/search) or select an employee known to have no data in the current range. &gt; 2. Click Search. &gt; 3. Wait for table. &gt; 4. Verify results.</t>
+  </si>
+  <si>
+    <t>Need locator for employee filter and Search button. Verify table is empty or shows a "No data found" message.</t>
+  </si>
+  <si>
+    <t>The table displays no entries or a "No data found" message.</t>
+  </si>
+  <si>
+    <t>Filter by Date Range with No Data</t>
+  </si>
+  <si>
+    <t>Verify filtering by a valid range where no data exists shows no results</t>
+  </si>
+  <si>
+    <t>Start Date: [Date X], End Date: [Date Y] (where X &lt;= Y but no data exists)</t>
+  </si>
+  <si>
+    <t>1. Enter [Date X] and [Date Y] for a range with no expected data. &gt; 2. Click Search. &gt; 3. Wait for table. &gt; 4. Verify results.</t>
+  </si>
+  <si>
+    <t>Need locators for date fields and Search button. Need to verify table is empty or shows a "No data found" message.</t>
+  </si>
+  <si>
+    <t>General Table Search for Non-existent Keyword</t>
+  </si>
+  <si>
+    <t>Verify searching for text not in the table shows no results</t>
+  </si>
+  <si>
+    <t>Non-existent Keyword String</t>
+  </si>
+  <si>
+    <t>1. Enter a keyword that is not expected to be found in any table data. &gt; 2. Wait for table to filter. &gt; 3. Verify results.</t>
+  </si>
+  <si>
+    <t>Need locator for the "Search..." input box. Verify table is empty or shows a "No data found" message.</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>HOLDING</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -597,7 +857,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -633,11 +893,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -668,6 +943,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -981,28 +1271,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35553CC5-25AE-452F-8D19-194CDDE17139}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="63" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="63" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.54296875"/>
-    <col min="2" max="2" customWidth="true" width="14.7265625"/>
-    <col min="3" max="3" customWidth="true" width="20.7265625"/>
-    <col min="4" max="4" customWidth="true" width="26.36328125"/>
-    <col min="5" max="5" customWidth="true" width="17.0"/>
-    <col min="6" max="6" customWidth="true" width="21.54296875"/>
-    <col min="7" max="7" customWidth="true" width="30.453125"/>
-    <col min="8" max="8" customWidth="true" width="26.453125"/>
-    <col min="9" max="9" customWidth="true" width="17.54296875"/>
-    <col min="10" max="10" customWidth="true" width="17.7265625"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="30.42578125" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1040,7 +1330,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="51" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1072,11 +1362,11 @@
       <c r="K2" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L2" t="s" s="0">
+      <c r="L2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="51" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1108,11 +1398,11 @@
       <c r="K3" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L3" t="s" s="0">
+      <c r="L3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="51" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1144,11 +1434,11 @@
       <c r="K4" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L4" t="s" s="0">
+      <c r="L4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="51" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1180,11 +1470,11 @@
       <c r="K5" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L5" t="s" s="0">
+      <c r="L5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1216,11 +1506,11 @@
       <c r="K6" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L6" t="s" s="0">
+      <c r="L6" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="39" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1252,11 +1542,11 @@
       <c r="K7" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L7" t="s" s="0">
+      <c r="L7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="51" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1288,11 +1578,11 @@
       <c r="K8" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L8" t="s" s="0">
+      <c r="L8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="39" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1324,11 +1614,11 @@
       <c r="K9" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L9" t="s" s="0">
+      <c r="L9" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="26" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1360,11 +1650,11 @@
       <c r="K10" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L10" t="s" s="0">
+      <c r="L10" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="39" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1396,11 +1686,11 @@
       <c r="K11" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L11" t="s" s="0">
+      <c r="L11" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="39" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1432,11 +1722,11 @@
       <c r="K12" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L12" t="s" s="0">
+      <c r="L12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="76" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1471,7 +1761,7 @@
       <c r="L13" s="6"/>
       <c r="M13" s="7"/>
     </row>
-    <row r="14" spans="1:13" ht="63.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1506,7 +1796,7 @@
       <c r="L14" s="6"/>
       <c r="M14" s="7"/>
     </row>
-    <row r="15" spans="1:13" ht="76" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1541,7 +1831,7 @@
       <c r="L15" s="6"/>
       <c r="M15" s="7"/>
     </row>
-    <row r="16" spans="1:13" ht="88.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1576,7 +1866,7 @@
       <c r="L16" s="6"/>
       <c r="M16" s="7"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1590,7 +1880,7 @@
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1604,7 +1894,7 @@
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1618,7 +1908,7 @@
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1632,7 +1922,7 @@
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -1647,35 +1937,602 @@
       <c r="L21" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1" xr:uid="{35553CC5-25AE-452F-8D19-194CDDE17139}"/>
+  <autoFilter ref="A1:M1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EB0A856-CBCF-4229-9F35-64381543B43D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="29.5703125" customWidth="1"/>
+    <col min="8" max="8" width="28" customWidth="1"/>
+    <col min="9" max="9" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="27">
+        <v>21</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="L2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="27">
+        <v>22</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="L3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27">
+        <v>23</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="L4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="27">
+        <v>24</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="L5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27">
+        <v>25</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="L6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="27">
+        <v>26</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="L7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="27">
+        <v>27</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="L8" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="27">
+        <v>28</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="I9" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="L9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="27">
+        <v>29</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="L10" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="27">
+        <v>30</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="L11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27">
+        <v>31</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="L12" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="27">
+        <v>32</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>208</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>210</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="L13" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="27">
+        <v>33</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>216</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="L14" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="27">
+        <v>34</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="G15" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="H15" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="L15" t="s">
+        <v>223</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.54296875"/>
-    <col min="2" max="2" customWidth="true" width="14.7265625"/>
-    <col min="3" max="3" customWidth="true" width="20.7265625"/>
-    <col min="4" max="4" customWidth="true" width="26.36328125"/>
-    <col min="5" max="5" customWidth="true" width="17.0"/>
-    <col min="6" max="6" customWidth="true" width="21.54296875"/>
-    <col min="7" max="7" customWidth="true" width="30.453125"/>
-    <col min="8" max="8" customWidth="true" width="26.453125"/>
-    <col min="9" max="9" customWidth="true" width="17.54296875"/>
-    <col min="10" max="10" customWidth="true" width="17.7265625"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="30.42578125" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1713,7 +2570,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="38.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="39" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>16</v>
       </c>
@@ -1745,11 +2602,11 @@
       <c r="K2" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="L2" t="s" s="0">
+      <c r="L2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="63.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>17</v>
       </c>
@@ -1781,11 +2638,11 @@
       <c r="K3" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="L3" t="s" s="0">
+      <c r="L3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="88.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>18</v>
       </c>
@@ -1817,11 +2674,11 @@
       <c r="K4" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="L4" t="s" s="0">
+      <c r="L4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="76" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>19</v>
       </c>
@@ -1853,11 +2710,11 @@
       <c r="K5" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="L5" t="s" s="0">
+      <c r="L5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>20</v>
       </c>
@@ -1889,7 +2746,7 @@
       <c r="K6" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L6" t="s" s="0">
+      <c r="L6" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add JDBC to query data from DB
</commit_message>
<xml_diff>
--- a/src/test/resources/report_demo.xlsx
+++ b/src/test/resources/report_demo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\test\Selenium\Selenium-Java\src\test\resources\"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="225">
   <si>
     <t>ID Test Case</t>
   </si>
@@ -757,11 +757,15 @@
   <si>
     <t>HOLDING</t>
   </si>
+  <si>
+    <t>FAIL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1280,16 +1284,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" customWidth="1"/>
-    <col min="7" max="7" width="30.42578125" customWidth="1"/>
-    <col min="8" max="8" width="26.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.5703125"/>
+    <col min="2" max="2" customWidth="true" width="14.7109375"/>
+    <col min="3" max="3" customWidth="true" width="20.7109375"/>
+    <col min="4" max="4" customWidth="true" width="26.42578125"/>
+    <col min="5" max="5" customWidth="true" width="17.0"/>
+    <col min="6" max="6" customWidth="true" width="21.5703125"/>
+    <col min="7" max="7" customWidth="true" width="30.42578125"/>
+    <col min="8" max="8" customWidth="true" width="26.42578125"/>
+    <col min="9" max="9" customWidth="true" width="17.5703125"/>
+    <col min="10" max="10" customWidth="true" width="17.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1362,7 +1366,7 @@
       <c r="K2" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -1398,7 +1402,7 @@
       <c r="K3" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -1434,7 +1438,7 @@
       <c r="K4" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -1470,7 +1474,7 @@
       <c r="K5" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -1506,7 +1510,7 @@
       <c r="K6" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -1542,7 +1546,7 @@
       <c r="K7" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -1578,7 +1582,7 @@
       <c r="K8" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -1614,7 +1618,7 @@
       <c r="K9" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -1650,7 +1654,7 @@
       <c r="K10" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -1686,7 +1690,7 @@
       <c r="K11" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -1722,7 +1726,7 @@
       <c r="K12" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -1953,13 +1957,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="29.5703125" customWidth="1"/>
-    <col min="8" max="8" width="28" customWidth="1"/>
-    <col min="9" max="9" width="26" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="23.85546875"/>
+    <col min="4" max="4" customWidth="true" width="27.140625"/>
+    <col min="5" max="5" customWidth="true" width="21.7109375"/>
+    <col min="6" max="6" customWidth="true" width="18.5703125"/>
+    <col min="7" max="7" customWidth="true" width="29.5703125"/>
+    <col min="8" max="8" customWidth="true" width="28.0"/>
+    <col min="9" max="9" customWidth="true" width="26.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2032,7 +2036,7 @@
       <c r="K2" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -2068,7 +2072,7 @@
       <c r="K3" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -2104,7 +2108,7 @@
       <c r="K4" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -2140,7 +2144,7 @@
       <c r="K5" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -2176,7 +2180,7 @@
       <c r="K6" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" t="s" s="0">
         <v>223</v>
       </c>
     </row>
@@ -2212,7 +2216,7 @@
       <c r="K7" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" t="s" s="0">
         <v>223</v>
       </c>
     </row>
@@ -2248,7 +2252,7 @@
       <c r="K8" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" t="s" s="0">
         <v>223</v>
       </c>
     </row>
@@ -2284,7 +2288,7 @@
       <c r="K9" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" t="s" s="0">
         <v>223</v>
       </c>
     </row>
@@ -2320,7 +2324,7 @@
       <c r="K10" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" t="s" s="0">
         <v>223</v>
       </c>
     </row>
@@ -2356,7 +2360,7 @@
       <c r="K11" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -2392,7 +2396,7 @@
       <c r="K12" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" t="s" s="0">
         <v>223</v>
       </c>
     </row>
@@ -2428,7 +2432,7 @@
       <c r="K13" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" t="s" s="0">
         <v>223</v>
       </c>
     </row>
@@ -2464,7 +2468,7 @@
       <c r="K14" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" t="s" s="0">
         <v>223</v>
       </c>
     </row>
@@ -2500,7 +2504,7 @@
       <c r="K15" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L15" t="s" s="0">
         <v>223</v>
       </c>
     </row>
@@ -2520,16 +2524,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" customWidth="1"/>
-    <col min="7" max="7" width="30.42578125" customWidth="1"/>
-    <col min="8" max="8" width="26.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.5703125"/>
+    <col min="2" max="2" customWidth="true" width="14.7109375"/>
+    <col min="3" max="3" customWidth="true" width="20.7109375"/>
+    <col min="4" max="4" customWidth="true" width="26.42578125"/>
+    <col min="5" max="5" customWidth="true" width="17.0"/>
+    <col min="6" max="6" customWidth="true" width="21.5703125"/>
+    <col min="7" max="7" customWidth="true" width="30.42578125"/>
+    <col min="8" max="8" customWidth="true" width="26.42578125"/>
+    <col min="9" max="9" customWidth="true" width="17.5703125"/>
+    <col min="10" max="10" customWidth="true" width="17.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2602,7 +2606,7 @@
       <c r="K2" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -2638,7 +2642,7 @@
       <c r="K3" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -2674,7 +2678,7 @@
       <c r="K4" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -2710,7 +2714,7 @@
       <c r="K5" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" t="s" s="0">
         <v>99</v>
       </c>
     </row>
@@ -2746,7 +2750,7 @@
       <c r="K6" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" t="s" s="0">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
check pagnition data on Manage Leave table
</commit_message>
<xml_diff>
--- a/src/test/resources/report_demo.xlsx
+++ b/src/test/resources/report_demo.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="232">
   <si>
     <t>ID Test Case</t>
   </si>
@@ -758,7 +758,29 @@
     <t>HOLDING</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <t>Data Table / Pagination</t>
+  </si>
+  <si>
+    <t>Pagination test</t>
+  </si>
+  <si>
+    <t>Check pagination when data is more than the maximum number of data that can be displayed on 1 page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home &gt; TimeSheet &gt; Manage Leave </t>
+  </si>
+  <si>
+    <t>Data table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Entries per page = 5
+2. Check items are displayed on table </t>
+  </si>
+  <si>
+    <t>Need to check total number of items and number of pages distributed</t>
+  </si>
+  <si>
+    <t>Total 11 items are divided into 3 pages, can be moved to other pages</t>
   </si>
 </sst>
 </file>
@@ -861,7 +883,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -912,11 +934,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -962,6 +995,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1949,10 +1989,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2506,6 +2546,38 @@
       </c>
       <c r="L15" t="s" s="0">
         <v>223</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="29">
+        <v>35</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>225</v>
+      </c>
+      <c r="D16" t="s" s="0">
+        <v>226</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="F16" t="s" s="0">
+        <v>228</v>
+      </c>
+      <c r="G16" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="H16" t="s" s="0">
+        <v>230</v>
+      </c>
+      <c r="I16" t="s" s="0">
+        <v>231</v>
+      </c>
+      <c r="K16" s="30" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change statement to preparedStatement to avoid SQL Injection
</commit_message>
<xml_diff>
--- a/src/test/resources/report_demo.xlsx
+++ b/src/test/resources/report_demo.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="233">
   <si>
     <t>ID Test Case</t>
   </si>
@@ -781,6 +781,9 @@
   </si>
   <si>
     <t>Total 11 items are divided into 3 pages, can be moved to other pages</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>

</xml_diff>